<commit_message>
Just finish the whole thing
</commit_message>
<xml_diff>
--- a/Electronics/Smartknob/BOM/Bill of Materials-Smartknob.xlsx
+++ b/Electronics/Smartknob/BOM/Bill of Materials-Smartknob.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mani\Documents\Projects\Smartknob\Electronics\Smartknob\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9CB093B6-8952-4013-9BB0-2F8443E7DA4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{EF27D7D8-A092-4801-8037-F65CF810EDC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2263" yWindow="2263" windowWidth="18514" windowHeight="11280" xr2:uid="{4559E90F-0686-4007-BCB8-F4A7B9FD9C1F}"/>
+    <workbookView xWindow="5863" yWindow="1071" windowWidth="18514" windowHeight="11280" xr2:uid="{160055F7-5538-496F-848A-66B077C08DD1}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-Smartknob" sheetId="1" r:id="rId1"/>
@@ -737,14 +737,14 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{953C134B-CFFB-497B-806E-98069A67E6E0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{979BAF1A-4023-4335-9A84-B0DD7AD0CEF6}">
   <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>